<commit_message>
NTR wip6 proposal for the first 3 fields.
</commit_message>
<xml_diff>
--- a/Revit-NTR-Exporter/NTR_CONFIG.xlsx
+++ b/Revit-NTR-Exporter/NTR_CONFIG.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="GENERAL" sheetId="1" r:id="rId1"/>
+    <sheet name="GEN" sheetId="1" r:id="rId1"/>
+    <sheet name="AUFT" sheetId="5" r:id="rId2"/>
+    <sheet name="TEXT" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>GEN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>TMONT</t>
   </si>
@@ -42,9 +41,6 @@
   </si>
   <si>
     <t>EN13480</t>
-  </si>
-  <si>
-    <t>AUFT</t>
   </si>
   <si>
     <t>TEXT</t>
@@ -409,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,61 +416,90 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>